<commit_message>
atualizacao para aps bacen
</commit_message>
<xml_diff>
--- a/database/pasta_sicaf/tabela_vazia.xlsx
+++ b/database/pasta_sicaf/tabela_vazia.xlsx
@@ -447,9 +447,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="100" customWidth="1" min="2" max="2"/>
-    <col width="150" customWidth="1" min="3" max="3"/>
-    <col width="200" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="100" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>